<commit_message>
ERD and Breakdown for Backend team
</commit_message>
<xml_diff>
--- a/haha/SPRINT.xlsx
+++ b/haha/SPRINT.xlsx
@@ -24,9 +24,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>BACK END</t>
-  </si>
-  <si>
     <t>send email</t>
   </si>
   <si>
@@ -85,15 +82,26 @@
   </si>
   <si>
     <t>api for email history (insert, get all(list), get by id, pagination)</t>
+  </si>
+  <si>
+    <t>BREAKDOWN FOR BACK END</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -172,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -194,6 +202,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,7 +510,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +522,13 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -524,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -533,13 +547,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -547,13 +561,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -561,33 +575,33 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -595,13 +609,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -609,20 +623,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,10 +649,10 @@
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -689,6 +703,9 @@
       <c r="D21" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>